<commit_message>
manuel proctoring almost done
</commit_message>
<xml_diff>
--- a/course info excel.xlsx
+++ b/course info excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atama\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atama\Desktop\Bilkent-TA-Mangement-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA45D85-F23E-428B-B80D-BA980F7BCFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170FE03A-9426-47F5-B017-82286E57B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12732" yWindow="1680" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Department</t>
   </si>
@@ -64,9 +64,6 @@
     <t>ENG200</t>
   </si>
   <si>
-    <t>Introduction to Programming</t>
-  </si>
-  <si>
     <t>Data Structures</t>
   </si>
   <si>
@@ -85,10 +82,34 @@
     <t>CS</t>
   </si>
   <si>
-    <t>CS101</t>
-  </si>
-  <si>
     <t>CS202</t>
+  </si>
+  <si>
+    <t>Academic Level</t>
+  </si>
+  <si>
+    <t>CS510</t>
+  </si>
+  <si>
+    <t>Advanced Machine Learning Algorithms</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>PhD Thesis II</t>
+  </si>
+  <si>
+    <t>ME601</t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
   </si>
 </sst>
 </file>
@@ -456,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,36 +504,42 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -523,8 +550,11 @@
       <c r="F3">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -532,19 +562,22 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -552,19 +585,22 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -572,7 +608,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -583,8 +619,11 @@
       <c r="F6">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -592,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -602,6 +641,32 @@
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>